<commit_message>
Se completa el archivo de entrada
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -1,22 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus Emiliano Reyes\OneDrive - GLOBAL HITSS\Escritorio\FW Interno Pruebas Bancs\FrameworkInterno\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716B9115-19CA-4CA7-86FE-E2462882DD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet 1 " sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Folio</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -43,14 +58,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -188,7 +212,6 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -199,27 +222,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -241,7 +268,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -299,7 +326,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -312,13 +339,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -330,70 +356,38 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Folio</v>
+    <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>465465465</v>
+    <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1212300002156</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A2"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>